<commit_message>
Botswana starting ideas and politics rework
</commit_message>
<xml_diff>
--- a/Modding resources/Politics/Parties.xlsx
+++ b/Modding resources/Politics/Parties.xlsx
@@ -3,17 +3,26 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CDEF46B-8150-48D6-B8EA-83C48690BDC5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21A62EFD-B5AE-413E-BA9F-6B06E6F0D4D5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Taul1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -204,6 +213,8 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
+Otlaadisa Koosaletse
+Gilson Saleshando
 Dumelang Saleshando</t>
         </r>
       </text>
@@ -772,6 +783,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="8" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="7" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="8" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -811,12 +828,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="8" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="7" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="8" xfId="2" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyvä" xfId="1" builtinId="26"/>
@@ -1102,7 +1113,7 @@
   <dimension ref="A2:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1118,16 +1129,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D2" s="42">
+      <c r="D2" s="48">
         <v>2000</v>
       </c>
-      <c r="E2" s="43"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="42">
+      <c r="E2" s="49"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="48">
         <v>2017</v>
       </c>
-      <c r="H2" s="43"/>
-      <c r="I2" s="44"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="50"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D3" s="6" t="s">
@@ -1235,10 +1246,10 @@
       <c r="I7" s="2"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="45" t="s">
+      <c r="B8" s="51" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="46"/>
+      <c r="C8" s="52"/>
       <c r="D8" s="20"/>
       <c r="E8" s="21"/>
       <c r="F8" s="22">
@@ -1372,10 +1383,10 @@
       <c r="I14" s="2"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="47" t="s">
+      <c r="B15" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="C15" s="48"/>
+      <c r="C15" s="54"/>
       <c r="D15" s="25"/>
       <c r="E15" s="26"/>
       <c r="F15" s="27">
@@ -1428,10 +1439,10 @@
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B18" s="49" t="s">
+      <c r="B18" s="55" t="s">
         <v>50</v>
       </c>
-      <c r="C18" s="50"/>
+      <c r="C18" s="56"/>
       <c r="D18" s="28"/>
       <c r="E18" s="29"/>
       <c r="F18" s="30">
@@ -1489,22 +1500,22 @@
       <c r="C21" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D21" s="53" t="s">
+      <c r="D21" s="40" t="s">
         <v>56</v>
       </c>
-      <c r="E21" s="53" t="s">
+      <c r="E21" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="F21" s="54">
+      <c r="F21" s="41">
         <v>42.3</v>
       </c>
-      <c r="G21" s="53" t="s">
+      <c r="G21" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="H21" s="55" t="s">
+      <c r="H21" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="I21" s="54">
+      <c r="I21" s="41">
         <v>52.7</v>
       </c>
     </row>
@@ -1535,13 +1546,13 @@
       <c r="C23" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="D23" s="56" t="s">
+      <c r="D23" s="43" t="s">
         <v>57</v>
       </c>
-      <c r="E23" s="57" t="s">
+      <c r="E23" s="44" t="s">
         <v>58</v>
       </c>
-      <c r="F23" s="58">
+      <c r="F23" s="45">
         <v>14.1</v>
       </c>
       <c r="G23" t="s">
@@ -1553,9 +1564,7 @@
       <c r="I23" s="2">
         <v>0</v>
       </c>
-      <c r="J23" s="38">
-        <v>2018</v>
-      </c>
+      <c r="J23" s="38"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
@@ -1628,10 +1637,10 @@
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B27" s="51" t="s">
+      <c r="B27" s="57" t="s">
         <v>51</v>
       </c>
-      <c r="C27" s="52"/>
+      <c r="C27" s="58"/>
       <c r="D27" s="31"/>
       <c r="E27" s="32"/>
       <c r="F27" s="33">
@@ -1746,10 +1755,10 @@
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B32" s="40" t="s">
+      <c r="B32" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="C32" s="41"/>
+      <c r="C32" s="47"/>
       <c r="D32" s="34"/>
       <c r="E32" s="35"/>
       <c r="F32" s="36">

</xml_diff>

<commit_message>
Spanish Portraits, Party Icons, and cleaned out old Spanish Submod Portraits
</commit_message>
<xml_diff>
--- a/Modding resources/Politics/Parties.xlsx
+++ b/Modding resources/Politics/Parties.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21A62EFD-B5AE-413E-BA9F-6B06E6F0D4D5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51F233C8-F3E0-4F71-83F2-05C688B9369A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="30" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Taul1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>Tekijä</author>
+    <author>Author</author>
   </authors>
   <commentList>
     <comment ref="E7" authorId="0" shapeId="0" xr:uid="{A4ADE693-6AB3-4B35-B4AB-AA4FA446C046}">
@@ -44,7 +44,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Tekijä:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -58,173 +58,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="E21" authorId="0" shapeId="0" xr:uid="{0DE32D80-EEFB-4E46-B642-F5509AFA5A37}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Tekijä:
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F21" authorId="0" shapeId="0" xr:uid="{9AA66E67-891B-4B5F-906B-068D4C93843F}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Tekijä:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-42,9</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H21" authorId="0" shapeId="0" xr:uid="{B965EB9D-96BF-41BD-AC4E-A3C1977A3256}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Tekijä:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Mokgweetsi Masisi</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I21" authorId="0" shapeId="0" xr:uid="{E1BBBA16-B61B-4BA0-8D48-42FA840CC755}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Tekijä:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-46,5</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E23" authorId="0" shapeId="0" xr:uid="{526ABE18-DC8C-40DE-9D67-4661AB197950}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Tekijä:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Gomolemo Motswaledi</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F23" authorId="0" shapeId="0" xr:uid="{8A97D6AD-FD7E-42E6-B661-50880B2B7AF3}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Tekijä:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-14,3</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E25" authorId="0" shapeId="0" xr:uid="{6505F9D3-8878-402A-A11D-641DDD8E4B6F}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Tekijä:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Otlaadisa Koosaletse
-Gilson Saleshando
-Dumelang Saleshando</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="102">
   <si>
     <t>Western_Autocracy</t>
   </si>
@@ -385,98 +224,158 @@
     <t>Nationalist</t>
   </si>
   <si>
-    <t>BDP - Botswana Democratic Party</t>
-  </si>
-  <si>
-    <t>Festus Mogae</t>
-  </si>
-  <si>
-    <t>Ian Khama</t>
-  </si>
-  <si>
-    <t>BDP (A-Team) - Botswana Democratic Party</t>
-  </si>
-  <si>
-    <t>BDP (Barata Phati) - Botswana Democratic Party</t>
-  </si>
-  <si>
-    <t>Daniel Kwelagobe</t>
-  </si>
-  <si>
-    <t>Ponatshego Kedikilwe</t>
-  </si>
-  <si>
-    <t>BNF - Botswana National Front</t>
-  </si>
-  <si>
-    <t>Otsweletse Moupo</t>
-  </si>
-  <si>
-    <t>Duma Boko</t>
-  </si>
-  <si>
-    <t>BCP - Botswana Congress Party</t>
-  </si>
-  <si>
-    <t>Michael Dingake</t>
-  </si>
-  <si>
-    <t>BAM - Botswana Alliance Movement</t>
-  </si>
-  <si>
-    <t>Ephraim Setshwaelo</t>
-  </si>
-  <si>
-    <t>MELS Movement of Botswana</t>
-  </si>
-  <si>
-    <t>Themba Joina</t>
-  </si>
-  <si>
-    <t>BPP - Botswana People's Party</t>
-  </si>
-  <si>
-    <t>Motlatsi Molapisi</t>
-  </si>
-  <si>
-    <t>UDC - Umbrella for Democratic Change</t>
-  </si>
-  <si>
-    <t>Alliance for Progressives</t>
-  </si>
-  <si>
-    <t>Ndaba Gaolathe</t>
-  </si>
-  <si>
-    <t>BMD - Botswana Movement for Democracy</t>
-  </si>
-  <si>
-    <t>ISBO - International Socialist Organization (Botswana)</t>
-  </si>
-  <si>
-    <t>Dikgosi</t>
-  </si>
-  <si>
-    <t>BDF - Botswana Defence Force</t>
-  </si>
-  <si>
-    <t>BWF - Botswana Workers Front</t>
-  </si>
-  <si>
-    <t>Mothusi Akanyang</t>
-  </si>
-  <si>
-    <t>Shawn Nthaile</t>
-  </si>
-  <si>
-    <t>Kgafela II</t>
+    <t>Partido Popular</t>
+  </si>
+  <si>
+    <t>Jose Aznar</t>
+  </si>
+  <si>
+    <t>Pablo Castado</t>
+  </si>
+  <si>
+    <t>Ciudadanos</t>
+  </si>
+  <si>
+    <t>Vox</t>
+  </si>
+  <si>
+    <t>Unidas Podemos</t>
+  </si>
+  <si>
+    <t>Juan Ramos Camarero</t>
+  </si>
+  <si>
+    <t>Carmelo Suarez</t>
+  </si>
+  <si>
+    <t>House of Bourbon/Carlists</t>
+  </si>
+  <si>
+    <t>House of Bourbon</t>
+  </si>
+  <si>
+    <t>Verdes</t>
+  </si>
+  <si>
+    <t>La Falange</t>
+  </si>
+  <si>
+    <t>Joaquin Almunia</t>
+  </si>
+  <si>
+    <t>Pedro Sanchez</t>
+  </si>
+  <si>
+    <t>King Juan Carlos</t>
+  </si>
+  <si>
+    <t>King Felipe VI</t>
+  </si>
+  <si>
+    <t>Partido Islamista</t>
+  </si>
+  <si>
+    <t>Alternativa Española</t>
+  </si>
+  <si>
+    <t>Partido Libertario</t>
+  </si>
+  <si>
+    <t>Daniel Martinez</t>
+  </si>
+  <si>
+    <t>Rafael López-Diéguez</t>
+  </si>
+  <si>
+    <t>Vicenta Rico</t>
+  </si>
+  <si>
+    <t>Joans Oms</t>
+  </si>
+  <si>
+    <t>Izquierda Unida</t>
+  </si>
+  <si>
+    <t>Francisco Frutos</t>
+  </si>
+  <si>
+    <t>Alberto Garzon</t>
+  </si>
+  <si>
+    <t>Jose Roberto</t>
+  </si>
+  <si>
+    <t>Santiago Abascal</t>
+  </si>
+  <si>
+    <t>Norberto Pico</t>
+  </si>
+  <si>
+    <t>Grupo Independiente Liberal</t>
+  </si>
+  <si>
+    <t>Jesus Gil</t>
+  </si>
+  <si>
+    <t>Centro Democraticio y Social</t>
+  </si>
+  <si>
+    <t>Mario Conde</t>
+  </si>
+  <si>
+    <t>Izquierda Revolucionaria</t>
+  </si>
+  <si>
+    <t>Estado Islámico de España</t>
+  </si>
+  <si>
+    <t>Francisca Cortés</t>
+  </si>
+  <si>
+    <t>Clan de La Paca</t>
+  </si>
+  <si>
+    <t>Plataforma de España 2000</t>
+  </si>
+  <si>
+    <t>Ejército de Tierra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Partido Comunista de España </t>
+  </si>
+  <si>
+    <t>Partido Socialista Obrero Español</t>
+  </si>
+  <si>
+    <t>Jose Luis Centella</t>
+  </si>
+  <si>
+    <t>Partido Comunista de Los Pueblos de España</t>
+  </si>
+  <si>
+    <t>King Juan Carlos/King Carlos Hugo</t>
+  </si>
+  <si>
+    <t>King Felipe VI/Carlos Javier</t>
+  </si>
+  <si>
+    <t>Alfonso Pardo</t>
+  </si>
+  <si>
+    <t>Albert Rivera</t>
+  </si>
+  <si>
+    <t>Francisco Javier</t>
+  </si>
+  <si>
+    <t>Pablo Igleasias Turrion</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -505,22 +404,8 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="9">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -557,18 +442,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -730,13 +605,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -783,12 +671,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="8" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="7" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="8" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -828,11 +710,13 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Hyvä" xfId="1" builtinId="26"/>
-    <cellStyle name="Neutraali" xfId="2" builtinId="28"/>
-    <cellStyle name="Normaali" xfId="0" builtinId="0"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1113,7 +997,7 @@
   <dimension ref="A2:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1121,24 +1005,24 @@
     <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="49.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.7109375" customWidth="1"/>
     <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="49.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.85546875" customWidth="1"/>
     <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D2" s="48">
+      <c r="D2" s="42">
         <v>2000</v>
       </c>
-      <c r="E2" s="49"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="48">
+      <c r="E2" s="43"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="42">
         <v>2017</v>
       </c>
-      <c r="H2" s="49"/>
-      <c r="I2" s="50"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="44"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D3" s="6" t="s">
@@ -1170,11 +1054,19 @@
       <c r="C4" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="24"/>
-      <c r="E4" s="23"/>
+      <c r="D4" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>67</v>
+      </c>
       <c r="F4" s="1"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="23"/>
+      <c r="G4" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="H4" s="24" t="s">
+        <v>68</v>
+      </c>
       <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1187,11 +1079,19 @@
       <c r="C5" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="37"/>
-      <c r="E5" s="17"/>
+      <c r="D5" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>54</v>
+      </c>
       <c r="F5" s="2"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="17"/>
+      <c r="G5" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="H5" s="38" t="s">
+        <v>55</v>
+      </c>
       <c r="I5" s="2"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1204,24 +1104,16 @@
       <c r="C6" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="E6" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="F6" s="2">
-        <v>4.3</v>
-      </c>
+      <c r="D6" s="24"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="2"/>
       <c r="G6" s="38" t="s">
-        <v>72</v>
-      </c>
-      <c r="H6" t="s">
-        <v>73</v>
-      </c>
-      <c r="I6" s="2">
-        <v>3.3</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="H6" s="38" t="s">
+        <v>99</v>
+      </c>
+      <c r="I6" s="2"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -1234,33 +1126,36 @@
         <v>27</v>
       </c>
       <c r="D7" s="37" t="s">
-        <v>60</v>
+        <v>93</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="F7" s="2">
-        <v>26.1</v>
-      </c>
-      <c r="G7" s="37"/>
+        <v>65</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="37" t="s">
+        <v>93</v>
+      </c>
+      <c r="H7" s="38" t="s">
+        <v>66</v>
+      </c>
       <c r="I7" s="2"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="51" t="s">
+      <c r="B8" s="45" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="52"/>
+      <c r="C8" s="46"/>
       <c r="D8" s="20"/>
       <c r="E8" s="21"/>
       <c r="F8" s="22">
         <f>SUM(F4:F7)</f>
-        <v>30.400000000000002</v>
+        <v>0</v>
       </c>
       <c r="G8" s="20"/>
       <c r="H8" s="21"/>
       <c r="I8" s="22">
         <f>SUM(I4:I7)</f>
-        <v>3.3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1274,23 +1169,21 @@
         <v>28</v>
       </c>
       <c r="D9" s="37" t="s">
-        <v>67</v>
+        <v>92</v>
       </c>
       <c r="E9" s="38" t="s">
-        <v>68</v>
+        <v>94</v>
       </c>
       <c r="F9" s="39">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="G9" s="37" t="s">
-        <v>67</v>
+        <v>92</v>
       </c>
       <c r="H9" s="38" t="s">
-        <v>68</v>
-      </c>
-      <c r="I9" s="2">
-        <v>0.1</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="I9" s="2"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -1302,17 +1195,19 @@
       <c r="C10" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="37" t="s">
-        <v>69</v>
-      </c>
-      <c r="E10" s="38" t="s">
-        <v>70</v>
-      </c>
-      <c r="F10" s="39">
-        <v>0</v>
-      </c>
-      <c r="G10" s="37"/>
-      <c r="H10" s="38"/>
+      <c r="D10" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="E10" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="H10" s="24" t="s">
+        <v>78</v>
+      </c>
       <c r="I10" s="2"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1325,10 +1220,14 @@
       <c r="C11" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="37"/>
+      <c r="D11" s="37" t="s">
+        <v>86</v>
+      </c>
       <c r="E11" s="38"/>
       <c r="F11" s="39"/>
-      <c r="G11" s="37"/>
+      <c r="G11" s="37" t="s">
+        <v>86</v>
+      </c>
       <c r="H11" s="17"/>
       <c r="I11" s="2"/>
     </row>
@@ -1383,21 +1282,21 @@
       <c r="I14" s="2"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="53" t="s">
+      <c r="B15" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="C15" s="54"/>
+      <c r="C15" s="48"/>
       <c r="D15" s="25"/>
       <c r="E15" s="26"/>
       <c r="F15" s="27">
         <f>SUM(F9:F14)</f>
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="G15" s="25"/>
       <c r="H15" s="26"/>
       <c r="I15" s="27">
         <f>SUM(I9:I14)</f>
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1427,33 +1326,33 @@
       <c r="C17" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="24"/>
+      <c r="D17" s="24" t="s">
+        <v>87</v>
+      </c>
       <c r="E17" s="17"/>
-      <c r="F17" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="G17" s="24"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="24" t="s">
+        <v>87</v>
+      </c>
       <c r="H17" s="17"/>
-      <c r="I17" s="2">
-        <v>0.1</v>
-      </c>
+      <c r="I17" s="2"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B18" s="55" t="s">
+      <c r="B18" s="49" t="s">
         <v>50</v>
       </c>
-      <c r="C18" s="56"/>
+      <c r="C18" s="50"/>
       <c r="D18" s="28"/>
       <c r="E18" s="29"/>
       <c r="F18" s="30">
         <f>SUM(F16:F17)</f>
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="G18" s="28"/>
       <c r="H18" s="29"/>
       <c r="I18" s="30">
         <f>SUM(I16:I17)</f>
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -1466,12 +1365,16 @@
       <c r="C19" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="D19" s="24"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="24"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="2"/>
+      <c r="D19" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
@@ -1484,11 +1387,11 @@
         <v>37</v>
       </c>
       <c r="D20" s="24"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="2"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
       <c r="G20" s="24"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="2"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
@@ -1500,24 +1403,20 @@
       <c r="C21" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D21" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="E21" s="40" t="s">
-        <v>54</v>
-      </c>
-      <c r="F21" s="41">
-        <v>42.3</v>
-      </c>
-      <c r="G21" s="40" t="s">
-        <v>53</v>
-      </c>
-      <c r="H21" s="42" t="s">
-        <v>55</v>
-      </c>
-      <c r="I21" s="41">
-        <v>52.7</v>
-      </c>
+      <c r="D21" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="E21" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="H21" t="s">
+        <v>73</v>
+      </c>
+      <c r="I21" s="24"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
@@ -1529,12 +1428,20 @@
       <c r="C22" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="D22" s="24"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="24"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="2"/>
+      <c r="D22" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="E22" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="F22" s="24"/>
+      <c r="G22" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="H22" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="I22" s="24"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
@@ -1546,24 +1453,20 @@
       <c r="C23" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="D23" s="43" t="s">
-        <v>57</v>
-      </c>
-      <c r="E23" s="44" t="s">
-        <v>58</v>
-      </c>
-      <c r="F23" s="45">
-        <v>14.1</v>
-      </c>
-      <c r="G23" t="s">
-        <v>74</v>
-      </c>
-      <c r="H23" t="s">
-        <v>59</v>
-      </c>
-      <c r="I23" s="2">
-        <v>0</v>
-      </c>
+      <c r="D23" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="E23" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="F23" s="24"/>
+      <c r="G23" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="H23" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="I23" s="24"/>
       <c r="J23" s="38"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -1576,12 +1479,20 @@
       <c r="C24" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="D24" s="24"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="24"/>
-      <c r="H24" s="17"/>
-      <c r="I24" s="2"/>
+      <c r="D24" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="E24" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="H24" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="I24" s="24"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
@@ -1593,24 +1504,16 @@
       <c r="C25" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="D25" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="E25" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="F25" s="2">
-        <v>12.9</v>
-      </c>
+      <c r="D25" s="24"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
       <c r="G25" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="H25" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="I25" s="2">
-        <v>43.7</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="H25" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="I25" s="24"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
@@ -1622,36 +1525,37 @@
       <c r="C26" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="D26" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="E26" s="17"/>
-      <c r="F26" s="2">
-        <v>0</v>
-      </c>
-      <c r="G26" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="I26" s="2">
-        <v>0</v>
-      </c>
+      <c r="D26" s="56" t="s">
+        <v>95</v>
+      </c>
+      <c r="E26" s="56" t="s">
+        <v>59</v>
+      </c>
+      <c r="F26" s="54"/>
+      <c r="G26" s="53" t="s">
+        <v>95</v>
+      </c>
+      <c r="H26" s="54" t="s">
+        <v>60</v>
+      </c>
+      <c r="I26" s="55"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B27" s="57" t="s">
+      <c r="B27" s="51" t="s">
         <v>51</v>
       </c>
-      <c r="C27" s="58"/>
+      <c r="C27" s="52"/>
       <c r="D27" s="31"/>
       <c r="E27" s="32"/>
       <c r="F27" s="33">
         <f>SUM(F19:F26)</f>
-        <v>69.3</v>
+        <v>0</v>
       </c>
       <c r="G27" s="31"/>
       <c r="H27" s="32"/>
       <c r="I27" s="33">
         <f>SUM(I19:I26)</f>
-        <v>96.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -1664,24 +1568,20 @@
       <c r="C28" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="D28" s="37" t="s">
-        <v>78</v>
-      </c>
-      <c r="E28" s="17" t="s">
+      <c r="D28" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="E28" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="F28" s="2">
-        <v>0</v>
-      </c>
-      <c r="G28" s="37" t="s">
-        <v>78</v>
-      </c>
-      <c r="H28" s="17" t="s">
+      <c r="F28" s="24"/>
+      <c r="G28" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="H28" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="I28" s="2">
-        <v>0</v>
-      </c>
+      <c r="I28" s="24"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
@@ -1693,12 +1593,20 @@
       <c r="C29" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="D29" s="37"/>
-      <c r="E29" s="17"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="37"/>
-      <c r="H29" s="17"/>
-      <c r="I29" s="2"/>
+      <c r="D29" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="E29" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="F29" s="24"/>
+      <c r="G29" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="H29" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="I29" s="24"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
@@ -1711,19 +1619,19 @@
         <v>44</v>
       </c>
       <c r="D30" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="E30" s="17"/>
-      <c r="F30" s="2">
-        <v>0</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="E30" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="F30" s="24"/>
       <c r="G30" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="H30" s="17"/>
-      <c r="I30" s="2">
-        <v>0</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="H30" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="I30" s="24"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31">
@@ -1735,51 +1643,47 @@
       <c r="C31" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="D31" t="s">
-        <v>76</v>
-      </c>
-      <c r="E31" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="F31" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="G31" t="s">
-        <v>76</v>
-      </c>
-      <c r="H31" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="I31" s="2">
-        <v>0.1</v>
-      </c>
+      <c r="D31" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="E31" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="F31" s="24"/>
+      <c r="G31" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="H31" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="I31" s="24"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B32" s="46" t="s">
+      <c r="B32" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="C32" s="47"/>
+      <c r="C32" s="41"/>
       <c r="D32" s="34"/>
       <c r="E32" s="35"/>
       <c r="F32" s="36">
         <f>SUM(F28:F31)</f>
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="G32" s="34"/>
       <c r="H32" s="35"/>
       <c r="I32" s="36">
         <f>SUM(I28:I31)</f>
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F33">
         <f>SUM(F8,F15,F18,F27,F32)</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="I33">
         <f>SUM(I8,I15,I18,I27,I32)</f>
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>